<commit_message>
Small manual edits in SeedData (remove duplicated header)
</commit_message>
<xml_diff>
--- a/data_raw/SeedData_combined.xlsx
+++ b/data_raw/SeedData_combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherryc/Desktop/mary gates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atorres\polybox - Agostina Torres (agostina.torres@usys.ethz.ch)@polybox.ethz.ch\ongoing projects\BeePriorityEffects\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65974133-F566-D442-BE48-D7F7C10FCBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665E4A44-3BA6-4FA8-8AD0-63C7A948323B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="37">
   <si>
     <t>HypRad</t>
   </si>
@@ -137,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -181,7 +181,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,18 +496,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I196"/>
+  <dimension ref="A1:I195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="21" width="15.1640625" customWidth="1"/>
+    <col min="1" max="21" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -533,7 +533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,7 +793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -3267,33 +3267,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="B106" s="2">
+        <v>41233</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
+      </c>
+      <c r="F106" s="1">
+        <v>4</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>31</v>
       </c>
@@ -3301,25 +3301,22 @@
         <v>41233</v>
       </c>
       <c r="C107" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F107" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
       </c>
-      <c r="H107" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+    </row>
+    <row r="108" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>31</v>
       </c>
@@ -3327,13 +3324,13 @@
         <v>41233</v>
       </c>
       <c r="C108" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D108" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F108" s="1">
         <v>0</v>
@@ -3342,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>31</v>
       </c>
@@ -3356,16 +3353,16 @@
         <v>2</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G109" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>31</v>
       </c>
@@ -3379,42 +3376,42 @@
         <v>2</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F110" s="1">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G110" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B111" s="2">
         <v>41233</v>
       </c>
       <c r="C111" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D111" s="1">
         <v>2</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F111" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G111" s="1">
         <v>0</v>
       </c>
-      <c r="H111" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+    </row>
+    <row r="112" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>34</v>
       </c>
@@ -3422,13 +3419,13 @@
         <v>41233</v>
       </c>
       <c r="C112" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F112" s="1">
         <v>0</v>
@@ -3437,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>34</v>
       </c>
@@ -3445,13 +3442,13 @@
         <v>41233</v>
       </c>
       <c r="C113" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D113" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1">
         <v>0</v>
@@ -3460,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>34</v>
       </c>
@@ -3471,10 +3468,10 @@
         <v>3</v>
       </c>
       <c r="D114" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F114" s="1">
         <v>0</v>
@@ -3482,8 +3479,11 @@
       <c r="G114" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="H114" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>34</v>
       </c>
@@ -3491,25 +3491,22 @@
         <v>41233</v>
       </c>
       <c r="C115" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D115" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F115" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115" s="1">
         <v>0</v>
       </c>
-      <c r="H115" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+    </row>
+    <row r="116" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>34</v>
       </c>
@@ -3523,16 +3520,16 @@
         <v>2</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F116" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G116" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -3540,13 +3537,13 @@
         <v>41233</v>
       </c>
       <c r="C117" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D117" s="1">
         <v>2</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F117" s="1">
         <v>0</v>
@@ -3555,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>34</v>
       </c>
@@ -3563,13 +3560,13 @@
         <v>41233</v>
       </c>
       <c r="C118" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D118" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F118" s="1">
         <v>0</v>
@@ -3578,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>34</v>
       </c>
@@ -3592,7 +3589,7 @@
         <v>1</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F119" s="1">
         <v>0</v>
@@ -3601,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>34</v>
       </c>
@@ -3612,10 +3609,10 @@
         <v>2</v>
       </c>
       <c r="D120" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F120" s="1">
         <v>0</v>
@@ -3624,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>34</v>
       </c>
@@ -3635,7 +3632,7 @@
         <v>2</v>
       </c>
       <c r="D121" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>6</v>
@@ -3647,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>34</v>
       </c>
@@ -3655,13 +3652,13 @@
         <v>41233</v>
       </c>
       <c r="C122" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D122" s="1">
         <v>1</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F122" s="1">
         <v>0</v>
@@ -3670,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>34</v>
       </c>
@@ -3684,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F123" s="1">
         <v>0</v>
@@ -3693,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>34</v>
       </c>
@@ -3701,22 +3698,22 @@
         <v>41233</v>
       </c>
       <c r="C124" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D124" s="1">
         <v>1</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F124" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G124" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>34</v>
       </c>
@@ -3733,13 +3730,13 @@
         <v>5</v>
       </c>
       <c r="F125" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>34</v>
       </c>
@@ -3756,13 +3753,16 @@
         <v>5</v>
       </c>
       <c r="F126" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="H126" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>34</v>
       </c>
@@ -3776,19 +3776,16 @@
         <v>1</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F127" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G127" s="1">
         <v>0</v>
       </c>
-      <c r="H127" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+    </row>
+    <row r="128" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>34</v>
       </c>
@@ -3805,13 +3802,13 @@
         <v>6</v>
       </c>
       <c r="F128" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G128" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>34</v>
       </c>
@@ -3825,16 +3822,16 @@
         <v>1</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F129" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G129" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>34</v>
       </c>
@@ -3851,13 +3848,13 @@
         <v>5</v>
       </c>
       <c r="F130" s="1">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G130" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>34</v>
       </c>
@@ -3871,16 +3868,16 @@
         <v>1</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F131" s="1">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="G131" s="1">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>34</v>
       </c>
@@ -3894,16 +3891,16 @@
         <v>1</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F132" s="1">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="G132" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>34</v>
       </c>
@@ -3920,13 +3917,13 @@
         <v>5</v>
       </c>
       <c r="F133" s="1">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="G133" s="1">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>34</v>
       </c>
@@ -3940,16 +3937,16 @@
         <v>1</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F134" s="1">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G134" s="1">
-        <v>1.1999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>34</v>
       </c>
@@ -3963,16 +3960,16 @@
         <v>1</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F135" s="1">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="G135" s="1">
-        <v>4.1999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>34</v>
       </c>
@@ -3989,13 +3986,13 @@
         <v>5</v>
       </c>
       <c r="F136" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G136" s="1">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>34</v>
       </c>
@@ -4003,22 +4000,22 @@
         <v>41233</v>
       </c>
       <c r="C137" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D137" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F137" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G137" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>34</v>
       </c>
@@ -4026,22 +4023,22 @@
         <v>41233</v>
       </c>
       <c r="C138" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D138" s="1">
         <v>2</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F138" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G138" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>34</v>
       </c>
@@ -4049,22 +4046,22 @@
         <v>41233</v>
       </c>
       <c r="C139" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D139" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F139" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G139" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>34</v>
       </c>
@@ -4072,22 +4069,22 @@
         <v>41233</v>
       </c>
       <c r="C140" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D140" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F140" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>34</v>
       </c>
@@ -4095,22 +4092,22 @@
         <v>41233</v>
       </c>
       <c r="C141" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D141" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F141" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G141" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>34</v>
       </c>
@@ -4121,34 +4118,34 @@
         <v>3</v>
       </c>
       <c r="D142" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E142" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B143" s="2">
+        <v>41238</v>
+      </c>
+      <c r="C143" s="1">
+        <v>2</v>
+      </c>
+      <c r="D143" s="1">
+        <v>1</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F142" s="1">
-        <v>2</v>
-      </c>
-      <c r="G142" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7">
-      <c r="A143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B143" s="2">
-        <v>41233</v>
-      </c>
-      <c r="C143" s="1">
-        <v>3</v>
-      </c>
-      <c r="D143" s="1">
-        <v>2</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F143" s="1">
         <v>0</v>
       </c>
@@ -4156,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>34</v>
       </c>
@@ -4170,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F144" s="1">
         <v>0</v>
@@ -4179,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>34</v>
       </c>
@@ -4193,16 +4190,16 @@
         <v>1</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F145" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G145" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>34</v>
       </c>
@@ -4210,22 +4207,22 @@
         <v>41238</v>
       </c>
       <c r="C146" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" s="1">
         <v>1</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F146" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G146" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>34</v>
       </c>
@@ -4233,13 +4230,13 @@
         <v>41238</v>
       </c>
       <c r="C147" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D147" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F147" s="1">
         <v>0</v>
@@ -4247,8 +4244,11 @@
       <c r="G147" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="H147" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>34</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>2</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F148" s="1">
         <v>0</v>
@@ -4274,7 +4274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>34</v>
       </c>
@@ -4285,10 +4285,10 @@
         <v>3</v>
       </c>
       <c r="D149" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F149" s="1">
         <v>0</v>
@@ -4296,11 +4296,8 @@
       <c r="G149" s="1">
         <v>0</v>
       </c>
-      <c r="H149" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8">
+    </row>
+    <row r="150" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>34</v>
       </c>
@@ -4314,16 +4311,16 @@
         <v>1</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F150" s="1">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G150" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>34</v>
       </c>
@@ -4337,16 +4334,16 @@
         <v>1</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F151" s="1">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="G151" s="1">
-        <v>4.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>34</v>
       </c>
@@ -4360,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F152" s="1">
         <v>0</v>
@@ -4369,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>34</v>
       </c>
@@ -4383,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F153" s="1">
         <v>0</v>
@@ -4392,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>34</v>
       </c>
@@ -4403,10 +4400,10 @@
         <v>3</v>
       </c>
       <c r="D154" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F154" s="1">
         <v>0</v>
@@ -4414,8 +4411,11 @@
       <c r="G154" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="H154" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>34</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>1</v>
@@ -4437,11 +4437,8 @@
       <c r="G155" s="1">
         <v>0</v>
       </c>
-      <c r="H155" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8">
+    </row>
+    <row r="156" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>34</v>
       </c>
@@ -4455,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F156" s="1">
         <v>0</v>
@@ -4464,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>34</v>
       </c>
@@ -4478,7 +4475,7 @@
         <v>1</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F157" s="1">
         <v>0</v>
@@ -4487,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>34</v>
       </c>
@@ -4498,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="D158" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>1</v>
@@ -4510,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>34</v>
       </c>
@@ -4518,13 +4515,13 @@
         <v>41238</v>
       </c>
       <c r="C159" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D159" s="1">
         <v>2</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F159" s="1">
         <v>0</v>
@@ -4533,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>34</v>
       </c>
@@ -4547,7 +4544,7 @@
         <v>2</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F160" s="1">
         <v>0</v>
@@ -4556,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>34</v>
       </c>
@@ -4564,22 +4561,22 @@
         <v>41238</v>
       </c>
       <c r="C161" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D161" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F161" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G161" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>34</v>
       </c>
@@ -4593,16 +4590,16 @@
         <v>1</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F162" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G162" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>34</v>
       </c>
@@ -4616,16 +4613,16 @@
         <v>1</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F163" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G163" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>34</v>
       </c>
@@ -4639,16 +4636,16 @@
         <v>1</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F164" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G164" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>34</v>
       </c>
@@ -4656,45 +4653,45 @@
         <v>41238</v>
       </c>
       <c r="C165" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D165" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F165" s="1">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="G165" s="1">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B166" s="2">
-        <v>41238</v>
+        <v>41239</v>
       </c>
       <c r="C166" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D166" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F166" s="1">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="G166" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>34</v>
       </c>
@@ -4702,22 +4699,22 @@
         <v>41239</v>
       </c>
       <c r="C167" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D167" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F167" s="1">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="G167" s="1">
-        <v>5.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>34</v>
       </c>
@@ -4731,7 +4728,7 @@
         <v>2</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F168" s="1">
         <v>0</v>
@@ -4740,7 +4737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>34</v>
       </c>
@@ -4748,7 +4745,7 @@
         <v>41239</v>
       </c>
       <c r="C169" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D169" s="1">
         <v>2</v>
@@ -4757,13 +4754,13 @@
         <v>3</v>
       </c>
       <c r="F169" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G169" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>34</v>
       </c>
@@ -4777,16 +4774,16 @@
         <v>2</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F170" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G170" s="1">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>34</v>
       </c>
@@ -4800,7 +4797,7 @@
         <v>2</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F171" s="1">
         <v>0</v>
@@ -4809,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>34</v>
       </c>
@@ -4823,16 +4820,16 @@
         <v>2</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F172" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G172" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>34</v>
       </c>
@@ -4840,22 +4837,22 @@
         <v>41239</v>
       </c>
       <c r="C173" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D173" s="1">
         <v>2</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F173" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G173" s="1">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>34</v>
       </c>
@@ -4869,16 +4866,16 @@
         <v>2</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F174" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G174" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>34</v>
       </c>
@@ -4892,7 +4889,7 @@
         <v>2</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F175" s="1">
         <v>0</v>
@@ -4901,7 +4898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>34</v>
       </c>
@@ -4909,22 +4906,22 @@
         <v>41239</v>
       </c>
       <c r="C176" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D176" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F176" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G176" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>34</v>
       </c>
@@ -4932,22 +4929,22 @@
         <v>41239</v>
       </c>
       <c r="C177" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D177" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F177" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G177" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>34</v>
       </c>
@@ -4961,7 +4958,7 @@
         <v>2</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F178" s="1">
         <v>0</v>
@@ -4970,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>34</v>
       </c>
@@ -4978,13 +4975,13 @@
         <v>41239</v>
       </c>
       <c r="C179" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D179" s="1">
         <v>2</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F179" s="1">
         <v>0</v>
@@ -4993,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>34</v>
       </c>
@@ -5007,7 +5004,7 @@
         <v>2</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F180" s="1">
         <v>0</v>
@@ -5016,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>34</v>
       </c>
@@ -5027,10 +5024,10 @@
         <v>1</v>
       </c>
       <c r="D181" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F181" s="1">
         <v>0</v>
@@ -5039,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>34</v>
       </c>
@@ -5053,7 +5050,7 @@
         <v>1</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F182" s="1">
         <v>0</v>
@@ -5062,7 +5059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>34</v>
       </c>
@@ -5076,7 +5073,7 @@
         <v>1</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F183" s="1">
         <v>0</v>
@@ -5085,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>34</v>
       </c>
@@ -5093,13 +5090,13 @@
         <v>41239</v>
       </c>
       <c r="C184" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D184" s="1">
         <v>1</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F184" s="1">
         <v>0</v>
@@ -5108,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>34</v>
       </c>
@@ -5116,13 +5113,13 @@
         <v>41239</v>
       </c>
       <c r="C185" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D185" s="1">
         <v>1</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F185" s="1">
         <v>0</v>
@@ -5131,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>34</v>
       </c>
@@ -5145,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F186" s="1">
         <v>0</v>
@@ -5154,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>34</v>
       </c>
@@ -5162,13 +5159,13 @@
         <v>41239</v>
       </c>
       <c r="C187" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D187" s="1">
         <v>1</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F187" s="1">
         <v>0</v>
@@ -5177,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>34</v>
       </c>
@@ -5185,13 +5182,13 @@
         <v>41239</v>
       </c>
       <c r="C188" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D188" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F188" s="1">
         <v>0</v>
@@ -5200,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>34</v>
       </c>
@@ -5208,13 +5205,13 @@
         <v>41239</v>
       </c>
       <c r="C189" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D189" s="1">
         <v>2</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F189" s="1">
         <v>0</v>
@@ -5223,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>34</v>
       </c>
@@ -5234,19 +5231,19 @@
         <v>3</v>
       </c>
       <c r="D190" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F190" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G190" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>34</v>
       </c>
@@ -5260,16 +5257,16 @@
         <v>1</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F191" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G191" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>34</v>
       </c>
@@ -5277,13 +5274,13 @@
         <v>41239</v>
       </c>
       <c r="C192" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F192" s="1">
         <v>0</v>
@@ -5292,7 +5289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>34</v>
       </c>
@@ -5309,13 +5306,13 @@
         <v>6</v>
       </c>
       <c r="F193" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G193" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>34</v>
       </c>
@@ -5329,16 +5326,16 @@
         <v>1</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F194" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G194" s="1">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>34</v>
       </c>
@@ -5352,35 +5349,12 @@
         <v>1</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F195" s="1">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G195" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7">
-      <c r="A196" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B196" s="2">
-        <v>41239</v>
-      </c>
-      <c r="C196" s="1">
-        <v>2</v>
-      </c>
-      <c r="D196" s="1">
-        <v>1</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F196" s="1">
-        <v>29</v>
-      </c>
-      <c r="G196" s="1">
         <v>3.0999999999999999E-3</v>
       </c>
     </row>

</xml_diff>